<commit_message>
Add multiplicative option for balance sheet metric mutations
</commit_message>
<xml_diff>
--- a/src/examples/scenarios/example_excel.xlsx
+++ b/src/examples/scenarios/example_excel.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\woute\repos\BankProjections\src\examples\scenarios\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F3761BA-BD67-4096-B3C7-63A038DA27EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CFBB26B-29AF-4187-BB2A-8E75B829AE59}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16776" xr2:uid="{3F47D940-11CC-4A58-ACDD-451DC7AB8FEE}"/>
   </bookViews>
@@ -36,14 +36,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>Relative</t>
   </si>
   <si>
-    <t>ItemType</t>
-  </si>
-  <si>
     <t>Mortgages</t>
   </si>
   <si>
@@ -66,6 +63,12 @@
   </si>
   <si>
     <t>Offset liquidity</t>
+  </si>
+  <si>
+    <t>Item_type</t>
+  </si>
+  <si>
+    <t>Multiplicative</t>
   </si>
 </sst>
 </file>
@@ -439,10 +442,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{865A046E-6CCA-4C12-800B-A91F40C91D45}">
-  <dimension ref="A1:D19"/>
+  <dimension ref="A1:D20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -453,25 +456,31 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" t="s">
         <v>3</v>
-      </c>
-      <c r="B1" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" t="s">
         <v>1</v>
-      </c>
-      <c r="B2" t="s">
-        <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B3" t="b">
+        <v>0</v>
+      </c>
+      <c r="C3" t="b">
+        <v>0</v>
+      </c>
+      <c r="D3" t="b">
         <v>1</v>
       </c>
     </row>
@@ -491,63 +500,73 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" t="b">
+        <v>0</v>
+      </c>
+      <c r="C5" t="b">
+        <v>0</v>
+      </c>
+      <c r="D5" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C6" t="s">
+        <v>4</v>
+      </c>
+      <c r="D6" t="s">
         <v>7</v>
-      </c>
-      <c r="B5" t="s">
-        <v>6</v>
-      </c>
-      <c r="C5" t="s">
-        <v>5</v>
-      </c>
-      <c r="D5" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A6" s="1">
-        <v>45777</v>
-      </c>
-      <c r="B6" s="2">
-        <v>0.25</v>
-      </c>
-      <c r="C6" s="2">
-        <v>0.01</v>
-      </c>
-      <c r="D6">
-        <v>100</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
-        <v>45808</v>
+        <v>45777</v>
       </c>
       <c r="B7" s="2">
         <v>0.25</v>
       </c>
       <c r="C7" s="2">
-        <v>0.02</v>
-      </c>
-      <c r="D7">
-        <v>200</v>
+        <v>0.01</v>
+      </c>
+      <c r="D7" s="2">
+        <v>0.5</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
+        <v>45808</v>
+      </c>
+      <c r="B8" s="2">
+        <v>0.25</v>
+      </c>
+      <c r="C8" s="2">
+        <v>0.02</v>
+      </c>
+      <c r="D8" s="2">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A9" s="1">
         <v>45838</v>
       </c>
-      <c r="B8" s="2">
+      <c r="B9" s="2">
         <v>0.3</v>
       </c>
-      <c r="C8" s="2">
+      <c r="C9" s="2">
         <v>0.03</v>
       </c>
-      <c r="D8">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A9" s="1"/>
-      <c r="C9" s="2"/>
+      <c r="D9" s="2">
+        <v>0.5</v>
+      </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" s="1"/>
@@ -588,6 +607,10 @@
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" s="1"/>
       <c r="C19" s="2"/>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A20" s="1"/>
+      <c r="C20" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Enhance BalanceSheetItem handling by adding counter item support; validate input values
</commit_message>
<xml_diff>
--- a/src/examples/scenarios/example_excel.xlsx
+++ b/src/examples/scenarios/example_excel.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\woute\repos\BankProjections\src\examples\scenarios\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CFBB26B-29AF-4187-BB2A-8E75B829AE59}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11C84F55-2CE1-487D-8DAF-D81D3A9B5E14}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16776" xr2:uid="{3F47D940-11CC-4A58-ACDD-451DC7AB8FEE}"/>
+    <workbookView xWindow="-132" yWindow="-132" windowWidth="30984" windowHeight="16824" xr2:uid="{3F47D940-11CC-4A58-ACDD-451DC7AB8FEE}"/>
   </bookViews>
   <sheets>
     <sheet name="metric overrides" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>Relative</t>
   </si>
@@ -62,13 +62,22 @@
     <t>Impairment</t>
   </si>
   <si>
-    <t>Offset liquidity</t>
-  </si>
-  <si>
     <t>Item_type</t>
   </si>
   <si>
     <t>Multiplicative</t>
+  </si>
+  <si>
+    <t>counter item type</t>
+  </si>
+  <si>
+    <t>Borrowings</t>
+  </si>
+  <si>
+    <t>Offset pnl</t>
+  </si>
+  <si>
+    <t>Agio</t>
   </si>
 </sst>
 </file>
@@ -442,10 +451,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{865A046E-6CCA-4C12-800B-A91F40C91D45}">
-  <dimension ref="A1:D20"/>
+  <dimension ref="A1:E21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -454,7 +463,7 @@
     <col min="2" max="2" width="20.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -462,17 +471,17 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="B3" t="b">
         <v>0</v>
@@ -483,8 +492,11 @@
       <c r="D3" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E3" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>0</v>
       </c>
@@ -497,10 +509,13 @@
       <c r="D4" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E4" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B5" t="b">
         <v>0</v>
@@ -511,88 +526,107 @@
       <c r="D5" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E5" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
         <v>6</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B7" t="s">
         <v>5</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C7" t="s">
         <v>4</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D7" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A7" s="1">
+      <c r="E7" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A8" s="1">
         <v>45777</v>
-      </c>
-      <c r="B7" s="2">
-        <v>0.25</v>
-      </c>
-      <c r="C7" s="2">
-        <v>0.01</v>
-      </c>
-      <c r="D7" s="2">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A8" s="1">
-        <v>45808</v>
       </c>
       <c r="B8" s="2">
         <v>0.25</v>
       </c>
       <c r="C8" s="2">
-        <v>0.02</v>
+        <v>0.01</v>
       </c>
       <c r="D8" s="2">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E8" s="2">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
-        <v>45838</v>
+        <v>45808</v>
       </c>
       <c r="B9" s="2">
-        <v>0.3</v>
+        <v>0.25</v>
       </c>
       <c r="C9" s="2">
-        <v>0.03</v>
+        <v>0.02</v>
       </c>
       <c r="D9" s="2">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A10" s="1"/>
-      <c r="C10" s="2"/>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E9" s="2">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A10" s="1">
+        <v>45838</v>
+      </c>
+      <c r="B10" s="2">
+        <v>0.3</v>
+      </c>
+      <c r="C10" s="2">
+        <v>0.03</v>
+      </c>
+      <c r="D10" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="E10" s="2">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" s="1"/>
       <c r="C11" s="2"/>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" s="1"/>
       <c r="C12" s="2"/>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" s="1"/>
       <c r="C13" s="2"/>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" s="1"/>
       <c r="C14" s="2"/>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" s="1"/>
       <c r="C15" s="2"/>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" s="1"/>
       <c r="C16" s="2"/>
     </row>
@@ -611,6 +645,10 @@
     <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" s="1"/>
       <c r="C20" s="2"/>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A21" s="1"/>
+      <c r="C21" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Support having multiple header rows
</commit_message>
<xml_diff>
--- a/src/examples/scenarios/example_excel.xlsx
+++ b/src/examples/scenarios/example_excel.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\woute\repos\BankProjections\src\examples\scenarios\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11C84F55-2CE1-487D-8DAF-D81D3A9B5E14}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F410EA6B-A548-493B-9DB2-0E5DD156CEA6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-132" yWindow="-132" windowWidth="30984" windowHeight="16824" xr2:uid="{3F47D940-11CC-4A58-ACDD-451DC7AB8FEE}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16776" xr2:uid="{3F47D940-11CC-4A58-ACDD-451DC7AB8FEE}"/>
   </bookViews>
   <sheets>
     <sheet name="metric overrides" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="16">
   <si>
     <t>Relative</t>
   </si>
@@ -78,6 +78,12 @@
   </si>
   <si>
     <t>Agio</t>
+  </si>
+  <si>
+    <t>BalanceSheetSide</t>
+  </si>
+  <si>
+    <t>Assets</t>
   </si>
 </sst>
 </file>
@@ -451,19 +457,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{865A046E-6CCA-4C12-800B-A91F40C91D45}">
-  <dimension ref="A1:E21"/>
+  <dimension ref="A1:F21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.5546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="20.21875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -471,7 +478,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>8</v>
       </c>
@@ -479,176 +486,188 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B3" t="s">
         <v>12</v>
       </c>
-      <c r="B3" t="b">
-        <v>0</v>
-      </c>
       <c r="C3" t="b">
         <v>0</v>
       </c>
       <c r="D3" t="b">
+        <v>0</v>
+      </c>
+      <c r="E3" t="b">
         <v>1</v>
       </c>
-      <c r="E3" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>0</v>
-      </c>
-      <c r="B4" t="b">
+      <c r="F3" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B4" t="s">
         <v>0</v>
       </c>
       <c r="C4" t="b">
         <v>0</v>
       </c>
       <c r="D4" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E4" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
+      <c r="F4" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B5" t="s">
         <v>9</v>
       </c>
-      <c r="B5" t="b">
-        <v>0</v>
-      </c>
       <c r="C5" t="b">
         <v>0</v>
       </c>
       <c r="D5" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E5" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
+      <c r="F5" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B6" t="s">
         <v>10</v>
       </c>
-      <c r="E6" t="s">
+      <c r="F6" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
+        <v>14</v>
+      </c>
+      <c r="B7" t="s">
         <v>6</v>
       </c>
-      <c r="B7" t="s">
+      <c r="C7" t="s">
         <v>5</v>
       </c>
-      <c r="C7" t="s">
+      <c r="D7" t="s">
         <v>4</v>
       </c>
-      <c r="D7" t="s">
+      <c r="E7" t="s">
         <v>7</v>
       </c>
-      <c r="E7" t="s">
+      <c r="F7" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A8" s="1">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>15</v>
+      </c>
+      <c r="B8" s="1">
         <v>45777</v>
       </c>
-      <c r="B8" s="2">
+      <c r="C8" s="2">
         <v>0.25</v>
       </c>
-      <c r="C8" s="2">
+      <c r="D8" s="2">
         <v>0.01</v>
-      </c>
-      <c r="D8" s="2">
-        <v>0.5</v>
       </c>
       <c r="E8" s="2">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A9" s="1">
+      <c r="F8" s="2">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>15</v>
+      </c>
+      <c r="B9" s="1">
         <v>45808</v>
       </c>
-      <c r="B9" s="2">
+      <c r="C9" s="2">
         <v>0.25</v>
       </c>
-      <c r="C9" s="2">
+      <c r="D9" s="2">
         <v>0.02</v>
-      </c>
-      <c r="D9" s="2">
-        <v>0.5</v>
       </c>
       <c r="E9" s="2">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A10" s="1">
+      <c r="F9" s="2">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>15</v>
+      </c>
+      <c r="B10" s="1">
         <v>45838</v>
       </c>
-      <c r="B10" s="2">
+      <c r="C10" s="2">
         <v>0.3</v>
       </c>
-      <c r="C10" s="2">
+      <c r="D10" s="2">
         <v>0.03</v>
-      </c>
-      <c r="D10" s="2">
-        <v>0.5</v>
       </c>
       <c r="E10" s="2">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A11" s="1"/>
-      <c r="C11" s="2"/>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A12" s="1"/>
-      <c r="C12" s="2"/>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A13" s="1"/>
-      <c r="C13" s="2"/>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A14" s="1"/>
-      <c r="C14" s="2"/>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A15" s="1"/>
-      <c r="C15" s="2"/>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A16" s="1"/>
-      <c r="C16" s="2"/>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A17" s="1"/>
-      <c r="C17" s="2"/>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A18" s="1"/>
-      <c r="C18" s="2"/>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A19" s="1"/>
-      <c r="C19" s="2"/>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A20" s="1"/>
-      <c r="C20" s="2"/>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A21" s="1"/>
-      <c r="C21" s="2"/>
+      <c r="F10" s="2">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B11" s="1"/>
+      <c r="D11" s="2"/>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B12" s="1"/>
+      <c r="D12" s="2"/>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B13" s="1"/>
+      <c r="D13" s="2"/>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B14" s="1"/>
+      <c r="D14" s="2"/>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B15" s="1"/>
+      <c r="D15" s="2"/>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B16" s="1"/>
+      <c r="D16" s="2"/>
+    </row>
+    <row r="17" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B17" s="1"/>
+      <c r="D17" s="2"/>
+    </row>
+    <row r="18" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B18" s="1"/>
+      <c r="D18" s="2"/>
+    </row>
+    <row r="19" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B19" s="1"/>
+      <c r="D19" s="2"/>
+    </row>
+    <row r="20" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B20" s="1"/>
+      <c r="D20" s="2"/>
+    </row>
+    <row r="21" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B21" s="1"/>
+      <c r="D21" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Refactor scenario handling to utilize TemplateRegistry for loading scenarios from folders; update Projection and Runoff classes to incorporate market rates in rule application.
</commit_message>
<xml_diff>
--- a/src/examples/scenarios/example_excel.xlsx
+++ b/src/examples/scenarios/example_excel.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\woute\repos\BankProjections\src\examples\scenarios\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F410EA6B-A548-493B-9DB2-0E5DD156CEA6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0669C327-30B8-4984-B653-E348F555BFB6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16776" xr2:uid="{3F47D940-11CC-4A58-ACDD-451DC7AB8FEE}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" activeTab="1" xr2:uid="{3F47D940-11CC-4A58-ACDD-451DC7AB8FEE}"/>
   </bookViews>
   <sheets>
     <sheet name="metric overrides" sheetId="1" r:id="rId1"/>
+    <sheet name="interest rates" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="37">
   <si>
     <t>Relative</t>
   </si>
@@ -84,6 +85,69 @@
   </si>
   <si>
     <t>Assets</t>
+  </si>
+  <si>
+    <t>InterestRates</t>
+  </si>
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Euribor</t>
+  </si>
+  <si>
+    <t>Tenor</t>
+  </si>
+  <si>
+    <t>Maturity</t>
+  </si>
+  <si>
+    <t>3m</t>
+  </si>
+  <si>
+    <t>Rate</t>
+  </si>
+  <si>
+    <t>Type</t>
+  </si>
+  <si>
+    <t>Spot</t>
+  </si>
+  <si>
+    <t>6m</t>
+  </si>
+  <si>
+    <t>Zero</t>
+  </si>
+  <si>
+    <t>1m</t>
+  </si>
+  <si>
+    <t>1y</t>
+  </si>
+  <si>
+    <t>20y</t>
+  </si>
+  <si>
+    <t>10y</t>
+  </si>
+  <si>
+    <t>30y</t>
+  </si>
+  <si>
+    <t>Swap</t>
+  </si>
+  <si>
+    <t>3M</t>
+  </si>
+  <si>
+    <t>1Y</t>
+  </si>
+  <si>
+    <t>10Y</t>
   </si>
 </sst>
 </file>
@@ -119,10 +183,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -459,18 +524,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{865A046E-6CCA-4C12-800B-A91F40C91D45}">
   <dimension ref="A1:F21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="15.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.5546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20.21875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.6328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.54296875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -478,7 +543,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>8</v>
       </c>
@@ -486,7 +551,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B3" t="s">
         <v>12</v>
       </c>
@@ -503,7 +568,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B4" t="s">
         <v>0</v>
       </c>
@@ -520,7 +585,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B5" t="s">
         <v>9</v>
       </c>
@@ -537,7 +602,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B6" t="s">
         <v>10</v>
       </c>
@@ -545,7 +610,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>14</v>
       </c>
@@ -565,7 +630,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>15</v>
       </c>
@@ -585,7 +650,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>15</v>
       </c>
@@ -605,7 +670,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>15</v>
       </c>
@@ -625,49 +690,254 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B11" s="1"/>
       <c r="D11" s="2"/>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B12" s="1"/>
       <c r="D12" s="2"/>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B13" s="1"/>
       <c r="D13" s="2"/>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B14" s="1"/>
       <c r="D14" s="2"/>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B15" s="1"/>
       <c r="D15" s="2"/>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B16" s="1"/>
       <c r="D16" s="2"/>
     </row>
-    <row r="17" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B17" s="1"/>
       <c r="D17" s="2"/>
     </row>
-    <row r="18" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B18" s="1"/>
       <c r="D18" s="2"/>
     </row>
-    <row r="19" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B19" s="1"/>
       <c r="D19" s="2"/>
     </row>
-    <row r="20" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B20" s="1"/>
       <c r="D20" s="2"/>
     </row>
-    <row r="21" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B21" s="1"/>
       <c r="D21" s="2"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{408AD00A-839B-4347-BBD4-5564B7B0FB9B}">
+  <dimension ref="A1:F11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="14.90625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E2" t="s">
+        <v>21</v>
+      </c>
+      <c r="F2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A3" s="1">
+        <v>44926</v>
+      </c>
+      <c r="B3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D3" t="s">
+        <v>22</v>
+      </c>
+      <c r="F3" s="3">
+        <v>3.0499999999999999E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A4" s="1">
+        <v>44926</v>
+      </c>
+      <c r="B4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C4" t="s">
+        <v>25</v>
+      </c>
+      <c r="D4" t="s">
+        <v>26</v>
+      </c>
+      <c r="F4" s="3">
+        <v>2.9499999999999998E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A5" s="1">
+        <v>44926</v>
+      </c>
+      <c r="B5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C5" t="s">
+        <v>27</v>
+      </c>
+      <c r="E5" t="s">
+        <v>28</v>
+      </c>
+      <c r="F5" s="3">
+        <v>3.1800000000000002E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A6" s="1">
+        <v>44926</v>
+      </c>
+      <c r="B6" t="s">
+        <v>19</v>
+      </c>
+      <c r="C6" t="s">
+        <v>27</v>
+      </c>
+      <c r="E6" t="s">
+        <v>29</v>
+      </c>
+      <c r="F6" s="3">
+        <v>2.86E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A7" s="1">
+        <v>44926</v>
+      </c>
+      <c r="B7" t="s">
+        <v>19</v>
+      </c>
+      <c r="C7" t="s">
+        <v>27</v>
+      </c>
+      <c r="E7" t="s">
+        <v>31</v>
+      </c>
+      <c r="F7" s="3">
+        <v>2.5499999999999998E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A8" s="1">
+        <v>44926</v>
+      </c>
+      <c r="B8" t="s">
+        <v>19</v>
+      </c>
+      <c r="C8" t="s">
+        <v>27</v>
+      </c>
+      <c r="E8" t="s">
+        <v>30</v>
+      </c>
+      <c r="F8" s="3">
+        <v>2.6499999999999999E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A9" s="1">
+        <v>44926</v>
+      </c>
+      <c r="B9" t="s">
+        <v>19</v>
+      </c>
+      <c r="C9" t="s">
+        <v>27</v>
+      </c>
+      <c r="E9" t="s">
+        <v>32</v>
+      </c>
+      <c r="F9" s="3">
+        <v>2.7E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A10" s="1">
+        <v>44926</v>
+      </c>
+      <c r="B10" t="s">
+        <v>19</v>
+      </c>
+      <c r="C10" t="s">
+        <v>33</v>
+      </c>
+      <c r="D10" t="s">
+        <v>34</v>
+      </c>
+      <c r="E10" t="s">
+        <v>35</v>
+      </c>
+      <c r="F10" s="3">
+        <v>2.8500000000000001E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A11" s="1">
+        <v>44926</v>
+      </c>
+      <c r="B11" t="s">
+        <v>19</v>
+      </c>
+      <c r="C11" t="s">
+        <v>33</v>
+      </c>
+      <c r="D11" t="s">
+        <v>34</v>
+      </c>
+      <c r="E11" t="s">
+        <v>36</v>
+      </c>
+      <c r="F11" s="3">
+        <v>2.5499999999999998E-2</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Add floating rate handling and update interest rate calculations in runoff and synthetic data modules
</commit_message>
<xml_diff>
--- a/src/examples/scenarios/example_excel.xlsx
+++ b/src/examples/scenarios/example_excel.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\woute\repos\BankProjections\src\examples\scenarios\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0669C327-30B8-4984-B653-E348F555BFB6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B40A9BB9-6C8B-4F57-B465-1270859514C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" activeTab="1" xr2:uid="{3F47D940-11CC-4A58-ACDD-451DC7AB8FEE}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16776" activeTab="1" xr2:uid="{3F47D940-11CC-4A58-ACDD-451DC7AB8FEE}"/>
   </bookViews>
   <sheets>
     <sheet name="metric overrides" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="37">
   <si>
     <t>Relative</t>
   </si>
@@ -741,10 +741,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{408AD00A-839B-4347-BBD4-5564B7B0FB9B}">
-  <dimension ref="A1:F11"/>
+  <dimension ref="A1:F20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="J13" sqref="J13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -939,6 +939,165 @@
         <v>2.5499999999999998E-2</v>
       </c>
     </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A12" s="1">
+        <v>46387</v>
+      </c>
+      <c r="B12" t="s">
+        <v>19</v>
+      </c>
+      <c r="C12" t="s">
+        <v>25</v>
+      </c>
+      <c r="D12" t="s">
+        <v>22</v>
+      </c>
+      <c r="F12" s="3">
+        <v>5.0500000000000003E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A13" s="1">
+        <v>46387</v>
+      </c>
+      <c r="B13" t="s">
+        <v>19</v>
+      </c>
+      <c r="C13" t="s">
+        <v>25</v>
+      </c>
+      <c r="D13" t="s">
+        <v>26</v>
+      </c>
+      <c r="F13" s="3">
+        <v>4.9500000000000002E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A14" s="1">
+        <v>46387</v>
+      </c>
+      <c r="B14" t="s">
+        <v>19</v>
+      </c>
+      <c r="C14" t="s">
+        <v>27</v>
+      </c>
+      <c r="E14" t="s">
+        <v>28</v>
+      </c>
+      <c r="F14" s="3">
+        <v>5.1799999999999999E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A15" s="1">
+        <v>46387</v>
+      </c>
+      <c r="B15" t="s">
+        <v>19</v>
+      </c>
+      <c r="C15" t="s">
+        <v>27</v>
+      </c>
+      <c r="E15" t="s">
+        <v>29</v>
+      </c>
+      <c r="F15" s="3">
+        <v>4.8600000000000004E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A16" s="1">
+        <v>46387</v>
+      </c>
+      <c r="B16" t="s">
+        <v>19</v>
+      </c>
+      <c r="C16" t="s">
+        <v>27</v>
+      </c>
+      <c r="E16" t="s">
+        <v>31</v>
+      </c>
+      <c r="F16" s="3">
+        <v>4.5499999999999999E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A17" s="1">
+        <v>46387</v>
+      </c>
+      <c r="B17" t="s">
+        <v>19</v>
+      </c>
+      <c r="C17" t="s">
+        <v>27</v>
+      </c>
+      <c r="E17" t="s">
+        <v>30</v>
+      </c>
+      <c r="F17" s="3">
+        <v>4.65E-2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A18" s="1">
+        <v>46387</v>
+      </c>
+      <c r="B18" t="s">
+        <v>19</v>
+      </c>
+      <c r="C18" t="s">
+        <v>27</v>
+      </c>
+      <c r="E18" t="s">
+        <v>32</v>
+      </c>
+      <c r="F18" s="3">
+        <v>4.7E-2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A19" s="1">
+        <v>46387</v>
+      </c>
+      <c r="B19" t="s">
+        <v>19</v>
+      </c>
+      <c r="C19" t="s">
+        <v>33</v>
+      </c>
+      <c r="D19" t="s">
+        <v>34</v>
+      </c>
+      <c r="E19" t="s">
+        <v>35</v>
+      </c>
+      <c r="F19" s="3">
+        <v>4.8500000000000001E-2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A20" s="1">
+        <v>46387</v>
+      </c>
+      <c r="B20" t="s">
+        <v>19</v>
+      </c>
+      <c r="C20" t="s">
+        <v>33</v>
+      </c>
+      <c r="D20" t="s">
+        <v>34</v>
+      </c>
+      <c r="E20" t="s">
+        <v>36</v>
+      </c>
+      <c r="F20" s="3">
+        <v>4.5499999999999999E-2</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Add tax handling to balance sheet and enhance related functionality
</commit_message>
<xml_diff>
--- a/src/examples/scenarios/example_excel.xlsx
+++ b/src/examples/scenarios/example_excel.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\woute\repos\BankProjections\src\examples\scenarios\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B40A9BB9-6C8B-4F57-B465-1270859514C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68BAC162-E9CC-4680-9808-D6FD06F41C85}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16776" activeTab="1" xr2:uid="{3F47D940-11CC-4A58-ACDD-451DC7AB8FEE}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16776" activeTab="2" xr2:uid="{3F47D940-11CC-4A58-ACDD-451DC7AB8FEE}"/>
   </bookViews>
   <sheets>
     <sheet name="metric overrides" sheetId="1" r:id="rId1"/>
     <sheet name="interest rates" sheetId="2" r:id="rId2"/>
+    <sheet name="tax" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="39">
   <si>
     <t>Relative</t>
   </si>
@@ -148,6 +149,12 @@
   </si>
   <si>
     <t>10Y</t>
+  </si>
+  <si>
+    <t>Tax Rate</t>
+  </si>
+  <si>
+    <t>Tax</t>
   </si>
 </sst>
 </file>
@@ -528,14 +535,14 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="15.6328125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.54296875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20.1796875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -543,7 +550,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>8</v>
       </c>
@@ -551,7 +558,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
         <v>12</v>
       </c>
@@ -568,7 +575,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
         <v>0</v>
       </c>
@@ -585,7 +592,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
         <v>9</v>
       </c>
@@ -602,7 +609,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
         <v>10</v>
       </c>
@@ -610,7 +617,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>14</v>
       </c>
@@ -630,7 +637,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>15</v>
       </c>
@@ -650,7 +657,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>15</v>
       </c>
@@ -670,7 +677,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>15</v>
       </c>
@@ -690,47 +697,47 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B11" s="1"/>
       <c r="D11" s="2"/>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B12" s="1"/>
       <c r="D12" s="2"/>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B13" s="1"/>
       <c r="D13" s="2"/>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B14" s="1"/>
       <c r="D14" s="2"/>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B15" s="1"/>
       <c r="D15" s="2"/>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B16" s="1"/>
       <c r="D16" s="2"/>
     </row>
-    <row r="17" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="17" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B17" s="1"/>
       <c r="D17" s="2"/>
     </row>
-    <row r="18" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="18" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B18" s="1"/>
       <c r="D18" s="2"/>
     </row>
-    <row r="19" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="19" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B19" s="1"/>
       <c r="D19" s="2"/>
     </row>
-    <row r="20" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="20" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B20" s="1"/>
       <c r="D20" s="2"/>
     </row>
-    <row r="21" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="21" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B21" s="1"/>
       <c r="D21" s="2"/>
     </row>
@@ -743,16 +750,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{408AD00A-839B-4347-BBD4-5564B7B0FB9B}">
   <dimension ref="A1:F20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J13" sqref="J13"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="14.90625" customWidth="1"/>
+    <col min="1" max="1" width="14.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -760,7 +767,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>17</v>
       </c>
@@ -780,7 +787,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>44926</v>
       </c>
@@ -797,7 +804,7 @@
         <v>3.0499999999999999E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>44926</v>
       </c>
@@ -814,7 +821,7 @@
         <v>2.9499999999999998E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>44926</v>
       </c>
@@ -831,7 +838,7 @@
         <v>3.1800000000000002E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>44926</v>
       </c>
@@ -848,7 +855,7 @@
         <v>2.86E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <v>44926</v>
       </c>
@@ -865,7 +872,7 @@
         <v>2.5499999999999998E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
         <v>44926</v>
       </c>
@@ -882,7 +889,7 @@
         <v>2.6499999999999999E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
         <v>44926</v>
       </c>
@@ -899,7 +906,7 @@
         <v>2.7E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
         <v>44926</v>
       </c>
@@ -919,7 +926,7 @@
         <v>2.8500000000000001E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
         <v>44926</v>
       </c>
@@ -939,7 +946,7 @@
         <v>2.5499999999999998E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
         <v>46387</v>
       </c>
@@ -956,7 +963,7 @@
         <v>5.0500000000000003E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" s="1">
         <v>46387</v>
       </c>
@@ -973,7 +980,7 @@
         <v>4.9500000000000002E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" s="1">
         <v>46387</v>
       </c>
@@ -990,7 +997,7 @@
         <v>5.1799999999999999E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" s="1">
         <v>46387</v>
       </c>
@@ -1007,7 +1014,7 @@
         <v>4.8600000000000004E-2</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" s="1">
         <v>46387</v>
       </c>
@@ -1024,7 +1031,7 @@
         <v>4.5499999999999999E-2</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" s="1">
         <v>46387</v>
       </c>
@@ -1041,7 +1048,7 @@
         <v>4.65E-2</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" s="1">
         <v>46387</v>
       </c>
@@ -1058,7 +1065,7 @@
         <v>4.7E-2</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" s="1">
         <v>46387</v>
       </c>
@@ -1078,7 +1085,7 @@
         <v>4.8500000000000001E-2</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20" s="1">
         <v>46387</v>
       </c>
@@ -1097,6 +1104,44 @@
       <c r="F20" s="3">
         <v>4.5499999999999999E-2</v>
       </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A677DDE5-DC58-4FA0-9231-0F203A0C4FFF}">
+  <dimension ref="A1:B4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D21" sqref="D21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="15.88671875" customWidth="1"/>
+    <col min="2" max="2" width="11.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B2" s="3">
+        <v>0.25700000000000001</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Add audit rule implementation
</commit_message>
<xml_diff>
--- a/src/examples/scenarios/example_excel.xlsx
+++ b/src/examples/scenarios/example_excel.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\woute\repos\BankProjections\src\examples\scenarios\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68BAC162-E9CC-4680-9808-D6FD06F41C85}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0AC42A3-7041-4A57-83FD-0FD84F23398F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16776" activeTab="2" xr2:uid="{3F47D940-11CC-4A58-ACDD-451DC7AB8FEE}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16776" activeTab="3" xr2:uid="{3F47D940-11CC-4A58-ACDD-451DC7AB8FEE}"/>
   </bookViews>
   <sheets>
     <sheet name="metric overrides" sheetId="1" r:id="rId1"/>
     <sheet name="interest rates" sheetId="2" r:id="rId2"/>
     <sheet name="tax" sheetId="3" r:id="rId3"/>
+    <sheet name="audit" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="44">
   <si>
     <t>Relative</t>
   </si>
@@ -155,6 +156,21 @@
   </si>
   <si>
     <t>Tax</t>
+  </si>
+  <si>
+    <t>Audit</t>
+  </si>
+  <si>
+    <t>closing month</t>
+  </si>
+  <si>
+    <t>audit month</t>
+  </si>
+  <si>
+    <t>TargetItemType</t>
+  </si>
+  <si>
+    <t>Retained earnings</t>
   </si>
 </sst>
 </file>
@@ -1114,8 +1130,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A677DDE5-DC58-4FA0-9231-0F203A0C4FFF}">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1146,4 +1162,54 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D314085B-29B2-4F1C-B0E6-FF11268580B0}">
+  <dimension ref="A1:B4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="12.109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B2">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>41</v>
+      </c>
+      <c r="B3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>42</v>
+      </c>
+      <c r="B4" t="s">
+        <v>43</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Add rule for dividend payment
</commit_message>
<xml_diff>
--- a/src/examples/scenarios/example_excel.xlsx
+++ b/src/examples/scenarios/example_excel.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\woute\repos\BankProjections\src\examples\scenarios\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0AC42A3-7041-4A57-83FD-0FD84F23398F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B0E4F0B-FD62-4179-B684-BD1130C18FE8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16776" activeTab="3" xr2:uid="{3F47D940-11CC-4A58-ACDD-451DC7AB8FEE}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" activeTab="4" xr2:uid="{3F47D940-11CC-4A58-ACDD-451DC7AB8FEE}"/>
   </bookViews>
   <sheets>
     <sheet name="metric overrides" sheetId="1" r:id="rId1"/>
     <sheet name="interest rates" sheetId="2" r:id="rId2"/>
     <sheet name="tax" sheetId="3" r:id="rId3"/>
     <sheet name="audit" sheetId="4" r:id="rId4"/>
+    <sheet name="dividend" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="50">
   <si>
     <t>Relative</t>
   </si>
@@ -171,13 +172,42 @@
   </si>
   <si>
     <t>Retained earnings</t>
+  </si>
+  <si>
+    <t>item</t>
+  </si>
+  <si>
+    <t>counter item</t>
+  </si>
+  <si>
+    <t>dividend</t>
+  </si>
+  <si>
+    <t>retained earnings</t>
+  </si>
+  <si>
+    <t>Quantity</t>
+  </si>
+  <si>
+    <t>offsetliquidity* Metric</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <numFmts count="2">
+    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="165" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+  </numFmts>
+  <fonts count="2" x14ac:knownFonts="1">
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -203,16 +233,19 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Comma" xfId="1" builtinId="3"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -548,7 +581,7 @@
   <dimension ref="A1:F21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1168,9 +1201,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D314085B-29B2-4F1C-B0E6-FF11268580B0}">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -1212,4 +1243,98 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{97DE07CC-039C-4C7A-989B-8D7D68DBC730}">
+  <dimension ref="A1:E6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="16.33203125" customWidth="1"/>
+    <col min="2" max="2" width="20.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.6640625" customWidth="1"/>
+    <col min="4" max="4" width="18.5546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.44140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>44</v>
+      </c>
+      <c r="B2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>45</v>
+      </c>
+      <c r="B3" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B4" t="s">
+        <v>44</v>
+      </c>
+      <c r="C4" t="s">
+        <v>45</v>
+      </c>
+      <c r="D4" t="s">
+        <v>49</v>
+      </c>
+      <c r="E4" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5" s="1">
+        <v>45930</v>
+      </c>
+      <c r="B5" t="s">
+        <v>46</v>
+      </c>
+      <c r="C5" t="s">
+        <v>47</v>
+      </c>
+      <c r="D5" t="b">
+        <v>0</v>
+      </c>
+      <c r="E5" s="4">
+        <v>-1000000</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A6" s="1">
+        <v>45991</v>
+      </c>
+      <c r="B6" t="s">
+        <v>46</v>
+      </c>
+      <c r="D6" t="b">
+        <v>1</v>
+      </c>
+      <c r="E6" s="4">
+        <v>1000000</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Add template for cost or income
</commit_message>
<xml_diff>
--- a/src/examples/scenarios/example_excel.xlsx
+++ b/src/examples/scenarios/example_excel.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\woute\repos\BankProjections\src\examples\scenarios\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE31F81D-9247-4B4E-A41A-34EED6890BC5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5896DB69-1562-4F0C-9053-1F9AA1668D07}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" activeTab="5" xr2:uid="{3F47D940-11CC-4A58-ACDD-451DC7AB8FEE}"/>
+    <workbookView xWindow="30612" yWindow="-108" windowWidth="30936" windowHeight="16776" activeTab="6" xr2:uid="{3F47D940-11CC-4A58-ACDD-451DC7AB8FEE}"/>
   </bookViews>
   <sheets>
     <sheet name="metric overrides" sheetId="1" r:id="rId1"/>
@@ -19,6 +19,7 @@
     <sheet name="audit" sheetId="4" r:id="rId4"/>
     <sheet name="dividend" sheetId="5" r:id="rId5"/>
     <sheet name="production" sheetId="6" r:id="rId6"/>
+    <sheet name="costs" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -41,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="57">
   <si>
     <t>Relative</t>
   </si>
@@ -200,6 +201,18 @@
   </si>
   <si>
     <t>Savings deposits</t>
+  </si>
+  <si>
+    <t>CostIncome</t>
+  </si>
+  <si>
+    <t>Amount</t>
+  </si>
+  <si>
+    <t>Rule</t>
+  </si>
+  <si>
+    <t>Project X</t>
   </si>
 </sst>
 </file>
@@ -810,7 +823,7 @@
   <dimension ref="A1:F20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:B1"/>
+      <selection activeCell="C38" sqref="C38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1174,7 +1187,7 @@
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1211,7 +1224,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D314085B-29B2-4F1C-B0E6-FF11268580B0}">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D24" sqref="D24"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -1351,8 +1366,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{204A3C72-8141-4CE1-9B29-33F3A1419413}">
   <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1425,4 +1440,53 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9C43755C-28A4-4F7D-9E15-F678C3B90758}">
+  <dimension ref="A1:C3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="13.453125" customWidth="1"/>
+    <col min="2" max="2" width="17.36328125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B2" t="s">
+        <v>55</v>
+      </c>
+      <c r="C2" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A3" s="1">
+        <v>46387</v>
+      </c>
+      <c r="B3" t="s">
+        <v>56</v>
+      </c>
+      <c r="C3">
+        <v>-10000</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Allow cost and income to have different P&L and cashflow timing
</commit_message>
<xml_diff>
--- a/src/examples/scenarios/example_excel.xlsx
+++ b/src/examples/scenarios/example_excel.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\woute\repos\BankProjections\src\examples\scenarios\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5896DB69-1562-4F0C-9053-1F9AA1668D07}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36D64B00-1D1A-4916-9E21-654698400084}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30612" yWindow="-108" windowWidth="30936" windowHeight="16776" activeTab="6" xr2:uid="{3F47D940-11CC-4A58-ACDD-451DC7AB8FEE}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" activeTab="6" xr2:uid="{3F47D940-11CC-4A58-ACDD-451DC7AB8FEE}"/>
   </bookViews>
   <sheets>
     <sheet name="metric overrides" sheetId="1" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="61">
   <si>
     <t>Relative</t>
   </si>
@@ -213,6 +213,18 @@
   </si>
   <si>
     <t>Project X</t>
+  </si>
+  <si>
+    <t>Project Y</t>
+  </si>
+  <si>
+    <t>PnL Start</t>
+  </si>
+  <si>
+    <t>PnL End</t>
+  </si>
+  <si>
+    <t>Project Z</t>
   </si>
 </sst>
 </file>
@@ -1444,19 +1456,20 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9C43755C-28A4-4F7D-9E15-F678C3B90758}">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="13.453125" customWidth="1"/>
     <col min="2" max="2" width="17.36328125" customWidth="1"/>
+    <col min="4" max="5" width="10.08984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -1464,7 +1477,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>17</v>
       </c>
@@ -1474,8 +1487,14 @@
       <c r="C2" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D2" t="s">
+        <v>58</v>
+      </c>
+      <c r="E2" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" s="1">
         <v>46387</v>
       </c>
@@ -1484,6 +1503,40 @@
       </c>
       <c r="C3">
         <v>-10000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A4" s="1">
+        <v>46752</v>
+      </c>
+      <c r="B4" t="s">
+        <v>57</v>
+      </c>
+      <c r="C4">
+        <v>-100000</v>
+      </c>
+      <c r="D4" s="1">
+        <v>46767</v>
+      </c>
+      <c r="E4" s="1">
+        <v>47026</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A5" s="1">
+        <v>45991</v>
+      </c>
+      <c r="B5" t="s">
+        <v>60</v>
+      </c>
+      <c r="C5">
+        <v>10000000</v>
+      </c>
+      <c r="D5" s="1">
+        <v>45703</v>
+      </c>
+      <c r="E5" s="1">
+        <v>45793</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Enhance balance sheet structure by introducing sub-item types for improved categorization and aggregation
</commit_message>
<xml_diff>
--- a/src/examples/scenarios/example_excel.xlsx
+++ b/src/examples/scenarios/example_excel.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\woute\repos\BankProjections\src\examples\scenarios\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36D64B00-1D1A-4916-9E21-654698400084}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55AD888F-F170-492F-A46F-8628595ACB22}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" activeTab="6" xr2:uid="{3F47D940-11CC-4A58-ACDD-451DC7AB8FEE}"/>
+    <workbookView xWindow="-90" yWindow="-90" windowWidth="19380" windowHeight="11460" activeTab="4" xr2:uid="{3F47D940-11CC-4A58-ACDD-451DC7AB8FEE}"/>
   </bookViews>
   <sheets>
     <sheet name="metric overrides" sheetId="1" r:id="rId1"/>
@@ -68,9 +68,6 @@
     <t>Impairment</t>
   </si>
   <si>
-    <t>Item_type</t>
-  </si>
-  <si>
     <t>Multiplicative</t>
   </si>
   <si>
@@ -170,9 +167,6 @@
     <t>audit month</t>
   </si>
   <si>
-    <t>TargetItemType</t>
-  </si>
-  <si>
     <t>Retained earnings</t>
   </si>
   <si>
@@ -197,9 +191,6 @@
     <t>Production</t>
   </si>
   <si>
-    <t>Reference Item Type</t>
-  </si>
-  <si>
     <t>Savings deposits</t>
   </si>
   <si>
@@ -225,6 +216,15 @@
   </si>
   <si>
     <t>Project Z</t>
+  </si>
+  <si>
+    <t>Sub_Item_type</t>
+  </si>
+  <si>
+    <t>TargetSubItemType</t>
+  </si>
+  <si>
+    <t>Reference Sub Item Type</t>
   </si>
 </sst>
 </file>
@@ -616,7 +616,7 @@
   <dimension ref="A1:F21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -636,7 +636,7 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>8</v>
+        <v>58</v>
       </c>
       <c r="B2" t="s">
         <v>1</v>
@@ -644,7 +644,7 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C3" t="b">
         <v>0</v>
@@ -678,7 +678,7 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C5" t="b">
         <v>0</v>
@@ -695,15 +695,15 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B6" t="s">
+        <v>9</v>
+      </c>
+      <c r="F6" t="s">
         <v>10</v>
-      </c>
-      <c r="F6" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B7" t="s">
         <v>6</v>
@@ -718,12 +718,12 @@
         <v>7</v>
       </c>
       <c r="F7" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B8" s="1">
         <v>45777</v>
@@ -743,7 +743,7 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B9" s="1">
         <v>45808</v>
@@ -763,7 +763,7 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B10" s="1">
         <v>45838</v>
@@ -835,7 +835,7 @@
   <dimension ref="A1:F20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C38" sqref="C38"/>
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -848,27 +848,27 @@
         <v>2</v>
       </c>
       <c r="B1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2" t="s">
         <v>17</v>
       </c>
-      <c r="B2" t="s">
-        <v>18</v>
-      </c>
       <c r="C2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E2" t="s">
         <v>20</v>
       </c>
-      <c r="E2" t="s">
-        <v>21</v>
-      </c>
       <c r="F2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.35">
@@ -876,13 +876,13 @@
         <v>44926</v>
       </c>
       <c r="B3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F3" s="3">
         <v>3.0499999999999999E-2</v>
@@ -893,13 +893,13 @@
         <v>44926</v>
       </c>
       <c r="B4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C4" t="s">
+        <v>24</v>
+      </c>
+      <c r="D4" t="s">
         <v>25</v>
-      </c>
-      <c r="D4" t="s">
-        <v>26</v>
       </c>
       <c r="F4" s="3">
         <v>2.9499999999999998E-2</v>
@@ -910,13 +910,13 @@
         <v>44926</v>
       </c>
       <c r="B5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C5" t="s">
+        <v>26</v>
+      </c>
+      <c r="E5" t="s">
         <v>27</v>
-      </c>
-      <c r="E5" t="s">
-        <v>28</v>
       </c>
       <c r="F5" s="3">
         <v>3.1800000000000002E-2</v>
@@ -927,13 +927,13 @@
         <v>44926</v>
       </c>
       <c r="B6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E6" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F6" s="3">
         <v>2.86E-2</v>
@@ -944,13 +944,13 @@
         <v>44926</v>
       </c>
       <c r="B7" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F7" s="3">
         <v>2.5499999999999998E-2</v>
@@ -961,13 +961,13 @@
         <v>44926</v>
       </c>
       <c r="B8" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C8" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F8" s="3">
         <v>2.6499999999999999E-2</v>
@@ -978,13 +978,13 @@
         <v>44926</v>
       </c>
       <c r="B9" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C9" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F9" s="3">
         <v>2.7E-2</v>
@@ -995,16 +995,16 @@
         <v>44926</v>
       </c>
       <c r="B10" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C10" t="s">
+        <v>32</v>
+      </c>
+      <c r="D10" t="s">
         <v>33</v>
       </c>
-      <c r="D10" t="s">
+      <c r="E10" t="s">
         <v>34</v>
-      </c>
-      <c r="E10" t="s">
-        <v>35</v>
       </c>
       <c r="F10" s="3">
         <v>2.8500000000000001E-2</v>
@@ -1015,16 +1015,16 @@
         <v>44926</v>
       </c>
       <c r="B11" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C11" t="s">
+        <v>32</v>
+      </c>
+      <c r="D11" t="s">
         <v>33</v>
       </c>
-      <c r="D11" t="s">
-        <v>34</v>
-      </c>
       <c r="E11" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F11" s="3">
         <v>2.5499999999999998E-2</v>
@@ -1035,13 +1035,13 @@
         <v>46387</v>
       </c>
       <c r="B12" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C12" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D12" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F12" s="3">
         <v>5.0500000000000003E-2</v>
@@ -1052,13 +1052,13 @@
         <v>46387</v>
       </c>
       <c r="B13" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C13" t="s">
+        <v>24</v>
+      </c>
+      <c r="D13" t="s">
         <v>25</v>
-      </c>
-      <c r="D13" t="s">
-        <v>26</v>
       </c>
       <c r="F13" s="3">
         <v>4.9500000000000002E-2</v>
@@ -1069,13 +1069,13 @@
         <v>46387</v>
       </c>
       <c r="B14" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C14" t="s">
+        <v>26</v>
+      </c>
+      <c r="E14" t="s">
         <v>27</v>
-      </c>
-      <c r="E14" t="s">
-        <v>28</v>
       </c>
       <c r="F14" s="3">
         <v>5.1799999999999999E-2</v>
@@ -1086,13 +1086,13 @@
         <v>46387</v>
       </c>
       <c r="B15" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C15" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E15" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F15" s="3">
         <v>4.8600000000000004E-2</v>
@@ -1103,13 +1103,13 @@
         <v>46387</v>
       </c>
       <c r="B16" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C16" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E16" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F16" s="3">
         <v>4.5499999999999999E-2</v>
@@ -1120,13 +1120,13 @@
         <v>46387</v>
       </c>
       <c r="B17" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C17" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E17" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F17" s="3">
         <v>4.65E-2</v>
@@ -1137,13 +1137,13 @@
         <v>46387</v>
       </c>
       <c r="B18" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C18" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E18" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F18" s="3">
         <v>4.7E-2</v>
@@ -1154,16 +1154,16 @@
         <v>46387</v>
       </c>
       <c r="B19" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C19" t="s">
+        <v>32</v>
+      </c>
+      <c r="D19" t="s">
         <v>33</v>
       </c>
-      <c r="D19" t="s">
+      <c r="E19" t="s">
         <v>34</v>
-      </c>
-      <c r="E19" t="s">
-        <v>35</v>
       </c>
       <c r="F19" s="3">
         <v>4.8500000000000001E-2</v>
@@ -1174,16 +1174,16 @@
         <v>46387</v>
       </c>
       <c r="B20" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C20" t="s">
+        <v>32</v>
+      </c>
+      <c r="D20" t="s">
         <v>33</v>
       </c>
-      <c r="D20" t="s">
-        <v>34</v>
-      </c>
       <c r="E20" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F20" s="3">
         <v>4.5499999999999999E-2</v>
@@ -1213,12 +1213,12 @@
         <v>2</v>
       </c>
       <c r="B1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B2" s="3">
         <v>0.25700000000000001</v>
@@ -1237,7 +1237,7 @@
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D24" sqref="D24"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1250,12 +1250,12 @@
         <v>2</v>
       </c>
       <c r="B1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B2">
         <v>12</v>
@@ -1263,7 +1263,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B3">
         <v>5</v>
@@ -1271,10 +1271,10 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>42</v>
+        <v>59</v>
       </c>
       <c r="B4" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
   </sheetData>
@@ -1286,7 +1286,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{97DE07CC-039C-4C7A-989B-8D7D68DBC730}">
   <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -1307,35 +1309,35 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
+        <v>42</v>
+      </c>
+      <c r="B2" t="s">
         <v>44</v>
-      </c>
-      <c r="B2" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
+        <v>43</v>
+      </c>
+      <c r="B3" t="s">
         <v>45</v>
-      </c>
-      <c r="B3" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B4" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C4" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D4" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="E4" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.35">
@@ -1343,10 +1345,10 @@
         <v>45930</v>
       </c>
       <c r="B5" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C5" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D5" t="b">
         <v>0</v>
@@ -1360,7 +1362,7 @@
         <v>45991</v>
       </c>
       <c r="B6" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D6" t="b">
         <v>1</v>
@@ -1379,7 +1381,7 @@
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1393,21 +1395,21 @@
         <v>2</v>
       </c>
       <c r="B1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B2" t="s">
-        <v>51</v>
+        <v>60</v>
       </c>
       <c r="C2" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.35">
@@ -1429,7 +1431,7 @@
         <v>46037</v>
       </c>
       <c r="B4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C4" s="4">
         <v>-100000000</v>
@@ -1443,7 +1445,7 @@
         <v>46902</v>
       </c>
       <c r="B5" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="C5" s="4">
         <v>-200000000</v>
@@ -1458,8 +1460,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9C43755C-28A4-4F7D-9E15-F678C3B90758}">
   <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1474,24 +1476,24 @@
         <v>2</v>
       </c>
       <c r="B1" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B2" t="s">
+        <v>52</v>
+      </c>
+      <c r="C2" t="s">
+        <v>51</v>
+      </c>
+      <c r="D2" t="s">
         <v>55</v>
       </c>
-      <c r="C2" t="s">
-        <v>54</v>
-      </c>
-      <c r="D2" t="s">
-        <v>58</v>
-      </c>
       <c r="E2" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">
@@ -1499,7 +1501,7 @@
         <v>46387</v>
       </c>
       <c r="B3" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="C3">
         <v>-10000</v>
@@ -1510,7 +1512,7 @@
         <v>46752</v>
       </c>
       <c r="B4" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="C4">
         <v>-100000</v>
@@ -1527,7 +1529,7 @@
         <v>45991</v>
       </c>
       <c r="B5" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="C5">
         <v>10000000</v>

</xml_diff>

<commit_message>
Make example numbers more realistic
</commit_message>
<xml_diff>
--- a/src/examples/scenarios/example_excel.xlsx
+++ b/src/examples/scenarios/example_excel.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\woute\repos\BankProjections\src\examples\scenarios\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55AD888F-F170-492F-A46F-8628595ACB22}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBE95B8F-6472-4E17-9AC7-1DA34FA5CBDB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-90" yWindow="-90" windowWidth="19380" windowHeight="11460" activeTab="4" xr2:uid="{3F47D940-11CC-4A58-ACDD-451DC7AB8FEE}"/>
+    <workbookView xWindow="30612" yWindow="-108" windowWidth="30936" windowHeight="16776" xr2:uid="{3F47D940-11CC-4A58-ACDD-451DC7AB8FEE}"/>
   </bookViews>
   <sheets>
     <sheet name="metric overrides" sheetId="1" r:id="rId1"/>
@@ -615,18 +615,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{865A046E-6CCA-4C12-800B-A91F40C91D45}">
   <dimension ref="A1:F21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="15.6328125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.54296875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20.1796875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="20.21875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -634,7 +634,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>58</v>
       </c>
@@ -642,7 +642,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
         <v>11</v>
       </c>
@@ -659,12 +659,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
         <v>0</v>
       </c>
       <c r="C4" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D4" t="b">
         <v>0</v>
@@ -676,7 +676,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
         <v>8</v>
       </c>
@@ -693,7 +693,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
         <v>9</v>
       </c>
@@ -701,7 +701,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>13</v>
       </c>
@@ -721,7 +721,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>14</v>
       </c>
@@ -729,19 +729,19 @@
         <v>45777</v>
       </c>
       <c r="C8" s="2">
-        <v>0.25</v>
+        <v>0.03</v>
       </c>
       <c r="D8" s="2">
         <v>0.01</v>
       </c>
       <c r="E8" s="2">
-        <v>0.5</v>
+        <v>0.2</v>
       </c>
       <c r="F8" s="2">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>14</v>
       </c>
@@ -749,19 +749,19 @@
         <v>45808</v>
       </c>
       <c r="C9" s="2">
-        <v>0.25</v>
+        <v>0.02</v>
       </c>
       <c r="D9" s="2">
         <v>0.02</v>
       </c>
       <c r="E9" s="2">
-        <v>0.5</v>
+        <v>0.2</v>
       </c>
       <c r="F9" s="2">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>14</v>
       </c>
@@ -769,59 +769,59 @@
         <v>45838</v>
       </c>
       <c r="C10" s="2">
-        <v>0.3</v>
+        <v>0.01</v>
       </c>
       <c r="D10" s="2">
         <v>0.03</v>
       </c>
       <c r="E10" s="2">
-        <v>0.5</v>
+        <v>0.2</v>
       </c>
       <c r="F10" s="2">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B11" s="1"/>
       <c r="D11" s="2"/>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B12" s="1"/>
       <c r="D12" s="2"/>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B13" s="1"/>
       <c r="D13" s="2"/>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B14" s="1"/>
       <c r="D14" s="2"/>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B15" s="1"/>
       <c r="D15" s="2"/>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B16" s="1"/>
       <c r="D16" s="2"/>
     </row>
-    <row r="17" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="17" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B17" s="1"/>
       <c r="D17" s="2"/>
     </row>
-    <row r="18" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="18" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B18" s="1"/>
       <c r="D18" s="2"/>
     </row>
-    <row r="19" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="19" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B19" s="1"/>
       <c r="D19" s="2"/>
     </row>
-    <row r="20" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="20" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B20" s="1"/>
       <c r="D20" s="2"/>
     </row>
-    <row r="21" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="21" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B21" s="1"/>
       <c r="D21" s="2"/>
     </row>
@@ -838,12 +838,12 @@
       <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="14.90625" customWidth="1"/>
+    <col min="1" max="1" width="14.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -851,7 +851,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>16</v>
       </c>
@@ -871,7 +871,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>44926</v>
       </c>
@@ -888,7 +888,7 @@
         <v>3.0499999999999999E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>44926</v>
       </c>
@@ -905,7 +905,7 @@
         <v>2.9499999999999998E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>44926</v>
       </c>
@@ -922,7 +922,7 @@
         <v>3.1800000000000002E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>44926</v>
       </c>
@@ -939,7 +939,7 @@
         <v>2.86E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <v>44926</v>
       </c>
@@ -956,7 +956,7 @@
         <v>2.5499999999999998E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
         <v>44926</v>
       </c>
@@ -973,7 +973,7 @@
         <v>2.6499999999999999E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
         <v>44926</v>
       </c>
@@ -990,7 +990,7 @@
         <v>2.7E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
         <v>44926</v>
       </c>
@@ -1010,7 +1010,7 @@
         <v>2.8500000000000001E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
         <v>44926</v>
       </c>
@@ -1030,7 +1030,7 @@
         <v>2.5499999999999998E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
         <v>46387</v>
       </c>
@@ -1047,7 +1047,7 @@
         <v>5.0500000000000003E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" s="1">
         <v>46387</v>
       </c>
@@ -1064,7 +1064,7 @@
         <v>4.9500000000000002E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" s="1">
         <v>46387</v>
       </c>
@@ -1081,7 +1081,7 @@
         <v>5.1799999999999999E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" s="1">
         <v>46387</v>
       </c>
@@ -1098,7 +1098,7 @@
         <v>4.8600000000000004E-2</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" s="1">
         <v>46387</v>
       </c>
@@ -1115,7 +1115,7 @@
         <v>4.5499999999999999E-2</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" s="1">
         <v>46387</v>
       </c>
@@ -1132,7 +1132,7 @@
         <v>4.65E-2</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" s="1">
         <v>46387</v>
       </c>
@@ -1149,7 +1149,7 @@
         <v>4.7E-2</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" s="1">
         <v>46387</v>
       </c>
@@ -1169,7 +1169,7 @@
         <v>4.8500000000000001E-2</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20" s="1">
         <v>46387</v>
       </c>
@@ -1202,13 +1202,13 @@
       <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="15.90625" customWidth="1"/>
-    <col min="2" max="2" width="11.6328125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.88671875" customWidth="1"/>
+    <col min="2" max="2" width="11.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -1216,7 +1216,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>36</v>
       </c>
@@ -1224,7 +1224,7 @@
         <v>0.25700000000000001</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="1"/>
     </row>
   </sheetData>
@@ -1240,12 +1240,12 @@
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12.08984375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -1253,7 +1253,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>39</v>
       </c>
@@ -1261,7 +1261,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>40</v>
       </c>
@@ -1269,7 +1269,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>59</v>
       </c>
@@ -1286,20 +1286,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{97DE07CC-039C-4C7A-989B-8D7D68DBC730}">
   <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="16.36328125" customWidth="1"/>
-    <col min="2" max="2" width="20.6328125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20.6328125" customWidth="1"/>
-    <col min="4" max="4" width="18.54296875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.453125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.33203125" customWidth="1"/>
+    <col min="2" max="2" width="20.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.6640625" customWidth="1"/>
+    <col min="4" max="4" width="18.5546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -1307,7 +1307,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>42</v>
       </c>
@@ -1315,7 +1315,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>43</v>
       </c>
@@ -1323,7 +1323,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>16</v>
       </c>
@@ -1340,7 +1340,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>45930</v>
       </c>
@@ -1354,10 +1354,10 @@
         <v>0</v>
       </c>
       <c r="E5" s="4">
-        <v>-1000000</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+        <v>-1000</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>45991</v>
       </c>
@@ -1368,7 +1368,7 @@
         <v>1</v>
       </c>
       <c r="E6" s="4">
-        <v>1000000</v>
+        <v>1000</v>
       </c>
     </row>
   </sheetData>
@@ -1381,16 +1381,16 @@
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="2" width="17.453125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.08984375" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="17.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -1398,7 +1398,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>16</v>
       </c>
@@ -1412,7 +1412,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>46295</v>
       </c>
@@ -1420,13 +1420,13 @@
         <v>1</v>
       </c>
       <c r="C3" s="4">
-        <v>10000000</v>
+        <v>10000</v>
       </c>
       <c r="D3">
         <v>30</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>46037</v>
       </c>
@@ -1434,13 +1434,13 @@
         <v>10</v>
       </c>
       <c r="C4" s="4">
-        <v>-100000000</v>
+        <v>-100000</v>
       </c>
       <c r="D4">
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>46902</v>
       </c>
@@ -1448,7 +1448,7 @@
         <v>49</v>
       </c>
       <c r="C5" s="4">
-        <v>-200000000</v>
+        <v>-200000</v>
       </c>
     </row>
   </sheetData>
@@ -1461,17 +1461,17 @@
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="13.453125" customWidth="1"/>
-    <col min="2" max="2" width="17.36328125" customWidth="1"/>
-    <col min="4" max="5" width="10.08984375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.44140625" customWidth="1"/>
+    <col min="2" max="2" width="17.33203125" customWidth="1"/>
+    <col min="4" max="5" width="10.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -1479,7 +1479,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>16</v>
       </c>
@@ -1496,7 +1496,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>46387</v>
       </c>
@@ -1504,10 +1504,10 @@
         <v>53</v>
       </c>
       <c r="C3">
-        <v>-10000</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+        <v>-10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>46752</v>
       </c>
@@ -1515,7 +1515,7 @@
         <v>54</v>
       </c>
       <c r="C4">
-        <v>-100000</v>
+        <v>-100</v>
       </c>
       <c r="D4" s="1">
         <v>46767</v>
@@ -1524,7 +1524,7 @@
         <v>47026</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>45991</v>
       </c>
@@ -1532,7 +1532,7 @@
         <v>57</v>
       </c>
       <c r="C5">
-        <v>10000000</v>
+        <v>10000</v>
       </c>
       <c r="D5" s="1">
         <v>45703</v>

</xml_diff>